<commit_message>
Prepping for grand simulation!
</commit_message>
<xml_diff>
--- a/Mirroring_Tuning_Map.xlsx
+++ b/Mirroring_Tuning_Map.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Cassidy.Northway\RemoteGit\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20558DD4-7C3A-4915-8A09-98635C92F8B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5076618-548F-4008-A849-0C5F90E19EB4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="18240" windowHeight="28440" xr2:uid="{0DB4FD3A-09F6-403A-AC61-2E950311FA18}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{0DB4FD3A-09F6-403A-AC61-2E950311FA18}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="124">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="127">
   <si>
     <t>Region</t>
   </si>
@@ -356,9 +356,6 @@
     <t>internal carotid L</t>
   </si>
   <si>
-    <t>arteries1</t>
-  </si>
-  <si>
     <t>superior mesenteric C</t>
   </si>
   <si>
@@ -368,15 +365,6 @@
     <t>hepatic artery proper C</t>
   </si>
   <si>
-    <t>arteries24</t>
-  </si>
-  <si>
-    <t>arteries2</t>
-  </si>
-  <si>
-    <t>arteries4</t>
-  </si>
-  <si>
     <t>inferior mesenteric C</t>
   </si>
   <si>
@@ -408,6 +396,27 @@
   </si>
   <si>
     <t>right_external_iliac_artery</t>
+  </si>
+  <si>
+    <t>2492, 2497, 2503</t>
+  </si>
+  <si>
+    <t>superior_mesenteric_artery</t>
+  </si>
+  <si>
+    <t>left_common_cartoid_artery</t>
+  </si>
+  <si>
+    <t>common_hepatic_artery</t>
+  </si>
+  <si>
+    <t>inferior_mesenteric_artery</t>
+  </si>
+  <si>
+    <t>Location</t>
+  </si>
+  <si>
+    <t>0, 0.5, -1</t>
   </si>
 </sst>
 </file>
@@ -765,21 +774,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B6E8BFF4-0D05-430E-8585-37D11465CBE2}">
-  <dimension ref="A1:I56"/>
+  <dimension ref="A1:K55"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F50" sqref="F50"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="F53" sqref="F53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="24.28515625" customWidth="1"/>
     <col min="2" max="2" width="19.140625" customWidth="1"/>
-    <col min="3" max="3" width="18.28515625" customWidth="1"/>
-    <col min="5" max="5" width="18.5703125" customWidth="1"/>
+    <col min="3" max="4" width="18.28515625" customWidth="1"/>
+    <col min="5" max="5" width="16.28515625" customWidth="1"/>
+    <col min="6" max="6" width="25.42578125" customWidth="1"/>
+    <col min="7" max="7" width="18.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -792,14 +803,20 @@
       <c r="E1" t="s">
         <v>104</v>
       </c>
-      <c r="H1" t="s">
+      <c r="F1" t="s">
+        <v>125</v>
+      </c>
+      <c r="G1" t="s">
+        <v>104</v>
+      </c>
+      <c r="J1" t="s">
         <v>88</v>
       </c>
-      <c r="I1" t="s">
+      <c r="K1" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -810,7 +827,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>5</v>
       </c>
@@ -818,447 +835,507 @@
         <v>17</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C5" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C6" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C7" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C8" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C9" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C10" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+        <v>24</v>
+      </c>
+      <c r="E10">
+        <v>1928</v>
+      </c>
+      <c r="F10">
+        <v>0.5</v>
+      </c>
+      <c r="G10" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C11" t="s">
-        <v>24</v>
-      </c>
-      <c r="E11" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B12" t="s">
+        <v>14</v>
+      </c>
+      <c r="C12" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B13" t="s">
+        <v>15</v>
+      </c>
+      <c r="C13" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>28</v>
+      </c>
+      <c r="B14" t="s">
+        <v>29</v>
+      </c>
+      <c r="C14" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B15" t="s">
+        <v>30</v>
+      </c>
+      <c r="C15" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B16" t="s">
+        <v>31</v>
+      </c>
+      <c r="C16" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="17" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B17" t="s">
+        <v>32</v>
+      </c>
+      <c r="C17" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="18" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B18" t="s">
+        <v>33</v>
+      </c>
+      <c r="C18" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="19" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B19" t="s">
+        <v>34</v>
+      </c>
+      <c r="C19" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="20" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B20" t="s">
+        <v>35</v>
+      </c>
+      <c r="C20" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="21" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B21" t="s">
+        <v>36</v>
+      </c>
+      <c r="C21" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="22" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B22" t="s">
+        <v>37</v>
+      </c>
+      <c r="C22" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="23" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B23" t="s">
+        <v>38</v>
+      </c>
+      <c r="C23" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="24" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B24" t="s">
+        <v>39</v>
+      </c>
+      <c r="C24" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="25" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B25" t="s">
+        <v>40</v>
+      </c>
+      <c r="C25" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="26" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B26" t="s">
+        <v>41</v>
+      </c>
+      <c r="C26" t="s">
+        <v>67</v>
+      </c>
+      <c r="E26">
+        <v>2113</v>
+      </c>
+      <c r="F26">
+        <v>0.5</v>
+      </c>
+      <c r="G26" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="27" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B27" t="s">
+        <v>42</v>
+      </c>
+      <c r="C27" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="28" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B28" t="s">
+        <v>43</v>
+      </c>
+      <c r="C28" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="29" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B29" t="s">
+        <v>44</v>
+      </c>
+      <c r="C29" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="30" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B30" t="s">
+        <v>45</v>
+      </c>
+      <c r="C30" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="31" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B31" t="s">
+        <v>46</v>
+      </c>
+      <c r="C31" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="32" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B32" t="s">
+        <v>47</v>
+      </c>
+      <c r="C32" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B33" t="s">
+        <v>117</v>
+      </c>
+      <c r="C33" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B34" t="s">
+        <v>48</v>
+      </c>
+      <c r="C34" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B35" t="s">
+        <v>49</v>
+      </c>
+      <c r="C35" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B36" t="s">
+        <v>50</v>
+      </c>
+      <c r="C36" t="s">
+        <v>76</v>
+      </c>
+      <c r="E36">
+        <v>2450</v>
+      </c>
+      <c r="F36">
+        <v>0.5</v>
+      </c>
+      <c r="G36" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B37" t="s">
+        <v>51</v>
+      </c>
+      <c r="C37" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B38" t="s">
+        <v>52</v>
+      </c>
+      <c r="C38" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B39" t="s">
+        <v>53</v>
+      </c>
+      <c r="C39" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B40" t="s">
+        <v>54</v>
+      </c>
+      <c r="C40" t="s">
+        <v>80</v>
+      </c>
+      <c r="E40">
+        <v>2379</v>
+      </c>
+      <c r="F40">
+        <v>0.5</v>
+      </c>
+      <c r="G40" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>81</v>
+      </c>
+      <c r="B41" t="s">
+        <v>82</v>
+      </c>
+      <c r="C41" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B42" t="s">
+        <v>85</v>
+      </c>
+      <c r="C42" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B43" t="s">
+        <v>86</v>
+      </c>
+      <c r="C43" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>90</v>
+      </c>
+      <c r="B44" t="s">
+        <v>95</v>
+      </c>
+      <c r="C44" t="s">
+        <v>119</v>
+      </c>
+      <c r="E44">
+        <v>2437</v>
+      </c>
+      <c r="F44">
+        <v>0.5</v>
+      </c>
+      <c r="G44" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B45" t="s">
+        <v>91</v>
+      </c>
+      <c r="C45" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B46" t="s">
+        <v>93</v>
+      </c>
+      <c r="C46" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B47" t="s">
+        <v>96</v>
+      </c>
+      <c r="C47" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B48" t="s">
+        <v>98</v>
+      </c>
+      <c r="C48" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="49" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B49" t="s">
+        <v>100</v>
+      </c>
+      <c r="C49" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="50" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B50" t="s">
+        <v>102</v>
+      </c>
+      <c r="C50" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="51" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B51" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B12" t="s">
-        <v>13</v>
-      </c>
-      <c r="C12" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B13" t="s">
-        <v>14</v>
-      </c>
-      <c r="C13" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B14" t="s">
-        <v>15</v>
-      </c>
-      <c r="C14" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>28</v>
-      </c>
-      <c r="B15" t="s">
-        <v>29</v>
-      </c>
-      <c r="C15" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B16" t="s">
-        <v>30</v>
-      </c>
-      <c r="C16" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="17" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B17" t="s">
-        <v>31</v>
-      </c>
-      <c r="C17" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="18" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B18" t="s">
-        <v>32</v>
-      </c>
-      <c r="C18" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="19" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B19" t="s">
-        <v>33</v>
-      </c>
-      <c r="C19" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="20" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B20" t="s">
-        <v>34</v>
-      </c>
-      <c r="C20" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="21" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B21" t="s">
-        <v>35</v>
-      </c>
-      <c r="C21" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="22" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B22" t="s">
-        <v>36</v>
-      </c>
-      <c r="C22" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="23" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B23" t="s">
-        <v>37</v>
-      </c>
-      <c r="C23" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="24" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B24" t="s">
-        <v>38</v>
-      </c>
-      <c r="C24" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="25" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B25" t="s">
-        <v>39</v>
-      </c>
-      <c r="C25" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="26" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B26" t="s">
-        <v>40</v>
-      </c>
-      <c r="C26" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="27" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B27" t="s">
-        <v>41</v>
-      </c>
-      <c r="C27" t="s">
-        <v>67</v>
-      </c>
-      <c r="E27" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="28" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B28" t="s">
-        <v>42</v>
-      </c>
-      <c r="C28" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="29" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B29" t="s">
-        <v>43</v>
-      </c>
-      <c r="C29" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="30" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B30" t="s">
-        <v>44</v>
-      </c>
-      <c r="C30" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="31" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B31" t="s">
-        <v>45</v>
-      </c>
-      <c r="C31" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="32" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B32" t="s">
-        <v>46</v>
-      </c>
-      <c r="C32" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B33" t="s">
-        <v>47</v>
-      </c>
-      <c r="C33" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B34" t="s">
+      <c r="C51" t="s">
+        <v>116</v>
+      </c>
+      <c r="E51">
+        <v>2512</v>
+      </c>
+      <c r="F51">
+        <v>0.5</v>
+      </c>
+      <c r="G51" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="52" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B52" t="s">
         <v>121</v>
       </c>
-      <c r="C34" t="s">
+      <c r="E52">
+        <v>852</v>
+      </c>
+      <c r="F52">
+        <v>0</v>
+      </c>
+      <c r="G52" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="53" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B53" t="s">
         <v>122</v>
       </c>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B35" t="s">
-        <v>48</v>
-      </c>
-      <c r="C35" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B36" t="s">
-        <v>49</v>
-      </c>
-      <c r="C36" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B37" t="s">
-        <v>50</v>
-      </c>
-      <c r="C37" t="s">
-        <v>76</v>
-      </c>
-      <c r="E37" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B38" t="s">
-        <v>51</v>
-      </c>
-      <c r="C38" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B39" t="s">
-        <v>52</v>
-      </c>
-      <c r="C39" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B40" t="s">
-        <v>53</v>
-      </c>
-      <c r="C40" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B41" t="s">
-        <v>54</v>
-      </c>
-      <c r="C41" t="s">
-        <v>80</v>
-      </c>
-      <c r="E41" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A42" t="s">
-        <v>81</v>
-      </c>
-      <c r="B42" t="s">
-        <v>82</v>
-      </c>
-      <c r="C42" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B43" t="s">
-        <v>85</v>
-      </c>
-      <c r="C43" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B44" t="s">
-        <v>86</v>
-      </c>
-      <c r="C44" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A45" t="s">
-        <v>90</v>
-      </c>
-      <c r="B45" t="s">
-        <v>95</v>
-      </c>
-      <c r="C45" t="s">
+      <c r="E53" t="s">
+        <v>120</v>
+      </c>
+      <c r="F53" t="s">
+        <v>126</v>
+      </c>
+      <c r="G53" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="54" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B54" t="s">
         <v>123</v>
       </c>
-      <c r="E45" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B46" t="s">
-        <v>91</v>
-      </c>
-      <c r="C46" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B47" t="s">
-        <v>93</v>
-      </c>
-      <c r="C47" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B48" t="s">
-        <v>96</v>
-      </c>
-      <c r="C48" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="49" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B49" t="s">
-        <v>98</v>
-      </c>
-      <c r="C49" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="50" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B50" t="s">
-        <v>100</v>
-      </c>
-      <c r="C50" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="51" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B51" t="s">
-        <v>102</v>
-      </c>
-      <c r="C51" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="52" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B52" t="s">
-        <v>119</v>
-      </c>
-      <c r="C52" t="s">
-        <v>120</v>
-      </c>
-      <c r="E52" t="s">
+      <c r="E54">
+        <v>2467</v>
+      </c>
+      <c r="F54">
+        <v>0.5</v>
+      </c>
+      <c r="G54" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="53" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B53" t="s">
-        <v>106</v>
-      </c>
-      <c r="E53" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="54" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B54" t="s">
-        <v>111</v>
-      </c>
-      <c r="E54" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="55" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="55" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B55" t="s">
-        <v>112</v>
-      </c>
-      <c r="E55" t="s">
+        <v>124</v>
+      </c>
+      <c r="E55">
+        <v>1031</v>
+      </c>
+      <c r="F55">
+        <v>0.5</v>
+      </c>
+      <c r="G55" t="s">
         <v>109</v>
-      </c>
-    </row>
-    <row r="56" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B56" t="s">
-        <v>110</v>
-      </c>
-      <c r="E56" t="s">
-        <v>113</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Revert "At home work"
This reverts commit 4d5271b19f1e6def0a92785ef816d6e92dc93773.
</commit_message>
<xml_diff>
--- a/Mirroring_Tuning_Map.xlsx
+++ b/Mirroring_Tuning_Map.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cbnor\Documents\Full Body Flow Model Project\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Cassidy.Northway\RemoteGit\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BAF001D7-2C6D-48A9-A692-0B50587BA0D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C1CEBF8-EBCF-43F5-A8A3-60838C8EA98E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975" xr2:uid="{0DB4FD3A-09F6-403A-AC61-2E950311FA18}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="18240" windowHeight="28440" xr2:uid="{0DB4FD3A-09F6-403A-AC61-2E950311FA18}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -481,9 +481,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Office 2013 - 2022">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -521,7 +521,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2013 - 2022">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -627,7 +627,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2013 - 2022">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -769,7 +769,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -779,21 +779,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B6E8BFF4-0D05-430E-8585-37D11465CBE2}">
   <dimension ref="A1:K57"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="B28" sqref="B28"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="24.265625" customWidth="1"/>
-    <col min="2" max="2" width="19.1328125" customWidth="1"/>
-    <col min="3" max="4" width="18.265625" customWidth="1"/>
-    <col min="5" max="5" width="16.265625" customWidth="1"/>
-    <col min="6" max="6" width="25.3984375" customWidth="1"/>
-    <col min="7" max="7" width="18.59765625" customWidth="1"/>
+    <col min="1" max="1" width="24.28515625" customWidth="1"/>
+    <col min="2" max="2" width="19.140625" customWidth="1"/>
+    <col min="3" max="4" width="18.28515625" customWidth="1"/>
+    <col min="5" max="5" width="16.28515625" customWidth="1"/>
+    <col min="6" max="6" width="25.42578125" customWidth="1"/>
+    <col min="7" max="7" width="18.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -819,7 +819,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -830,7 +830,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>5</v>
       </c>
@@ -838,7 +838,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>6</v>
       </c>
@@ -846,7 +846,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>7</v>
       </c>
@@ -854,7 +854,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>8</v>
       </c>
@@ -862,7 +862,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>9</v>
       </c>
@@ -870,7 +870,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
         <v>10</v>
       </c>
@@ -878,7 +878,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
         <v>11</v>
       </c>
@@ -886,7 +886,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
         <v>12</v>
       </c>
@@ -903,7 +903,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
         <v>13</v>
       </c>
@@ -911,7 +911,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
         <v>14</v>
       </c>
@@ -919,7 +919,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
         <v>15</v>
       </c>
@@ -927,7 +927,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>28</v>
       </c>
@@ -938,7 +938,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
         <v>30</v>
       </c>
@@ -946,7 +946,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
         <v>31</v>
       </c>
@@ -954,7 +954,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="17" spans="2:7" x14ac:dyDescent="0.45">
+    <row r="17" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
         <v>32</v>
       </c>
@@ -962,7 +962,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="18" spans="2:7" x14ac:dyDescent="0.45">
+    <row r="18" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
         <v>33</v>
       </c>
@@ -970,7 +970,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="19" spans="2:7" x14ac:dyDescent="0.45">
+    <row r="19" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
         <v>34</v>
       </c>
@@ -978,7 +978,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="20" spans="2:7" x14ac:dyDescent="0.45">
+    <row r="20" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
         <v>35</v>
       </c>
@@ -986,7 +986,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="21" spans="2:7" x14ac:dyDescent="0.45">
+    <row r="21" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
         <v>36</v>
       </c>
@@ -994,7 +994,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="22" spans="2:7" x14ac:dyDescent="0.45">
+    <row r="22" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
         <v>37</v>
       </c>
@@ -1002,7 +1002,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="23" spans="2:7" x14ac:dyDescent="0.45">
+    <row r="23" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
         <v>38</v>
       </c>
@@ -1010,7 +1010,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="24" spans="2:7" x14ac:dyDescent="0.45">
+    <row r="24" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B24" t="s">
         <v>39</v>
       </c>
@@ -1018,7 +1018,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="25" spans="2:7" x14ac:dyDescent="0.45">
+    <row r="25" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B25" t="s">
         <v>40</v>
       </c>
@@ -1026,7 +1026,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="26" spans="2:7" x14ac:dyDescent="0.45">
+    <row r="26" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B26" t="s">
         <v>41</v>
       </c>
@@ -1043,7 +1043,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="27" spans="2:7" x14ac:dyDescent="0.45">
+    <row r="27" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B27" t="s">
         <v>42</v>
       </c>
@@ -1051,7 +1051,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="28" spans="2:7" x14ac:dyDescent="0.45">
+    <row r="28" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B28" t="s">
         <v>43</v>
       </c>
@@ -1059,7 +1059,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="29" spans="2:7" x14ac:dyDescent="0.45">
+    <row r="29" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B29" t="s">
         <v>44</v>
       </c>
@@ -1067,7 +1067,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="30" spans="2:7" x14ac:dyDescent="0.45">
+    <row r="30" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B30" t="s">
         <v>45</v>
       </c>
@@ -1075,7 +1075,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="31" spans="2:7" x14ac:dyDescent="0.45">
+    <row r="31" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B31" t="s">
         <v>46</v>
       </c>
@@ -1083,7 +1083,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="32" spans="2:7" x14ac:dyDescent="0.45">
+    <row r="32" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B32" t="s">
         <v>47</v>
       </c>
@@ -1091,7 +1091,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B33" t="s">
         <v>117</v>
       </c>
@@ -1099,7 +1099,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B34" t="s">
         <v>48</v>
       </c>
@@ -1107,7 +1107,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B35" t="s">
         <v>49</v>
       </c>
@@ -1115,7 +1115,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B36" t="s">
         <v>50</v>
       </c>
@@ -1132,7 +1132,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B37" t="s">
         <v>51</v>
       </c>
@@ -1140,7 +1140,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B38" t="s">
         <v>52</v>
       </c>
@@ -1148,7 +1148,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B39" t="s">
         <v>53</v>
       </c>
@@ -1156,7 +1156,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B40" t="s">
         <v>54</v>
       </c>
@@ -1173,7 +1173,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>81</v>
       </c>
@@ -1184,7 +1184,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B42" t="s">
         <v>85</v>
       </c>
@@ -1192,7 +1192,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B43" t="s">
         <v>86</v>
       </c>
@@ -1200,7 +1200,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>90</v>
       </c>
@@ -1220,7 +1220,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B45" t="s">
         <v>91</v>
       </c>
@@ -1228,7 +1228,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B46" t="s">
         <v>93</v>
       </c>
@@ -1236,7 +1236,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B47" t="s">
         <v>96</v>
       </c>
@@ -1244,7 +1244,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B48" t="s">
         <v>98</v>
       </c>
@@ -1252,7 +1252,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="49" spans="2:7" x14ac:dyDescent="0.45">
+    <row r="49" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B49" t="s">
         <v>100</v>
       </c>
@@ -1260,7 +1260,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="50" spans="2:7" x14ac:dyDescent="0.45">
+    <row r="50" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B50" t="s">
         <v>102</v>
       </c>
@@ -1268,7 +1268,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="51" spans="2:7" x14ac:dyDescent="0.45">
+    <row r="51" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B51" t="s">
         <v>115</v>
       </c>
@@ -1285,7 +1285,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="52" spans="2:7" x14ac:dyDescent="0.45">
+    <row r="52" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B52" t="s">
         <v>120</v>
       </c>
@@ -1299,7 +1299,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="53" spans="2:7" x14ac:dyDescent="0.45">
+    <row r="53" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B53" t="s">
         <v>121</v>
       </c>
@@ -1313,7 +1313,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="54" spans="2:7" x14ac:dyDescent="0.45">
+    <row r="54" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B54" t="s">
         <v>121</v>
       </c>
@@ -1324,7 +1324,7 @@
         <v>0.75</v>
       </c>
     </row>
-    <row r="55" spans="2:7" x14ac:dyDescent="0.45">
+    <row r="55" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B55" t="s">
         <v>121</v>
       </c>
@@ -1335,7 +1335,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="56" spans="2:7" x14ac:dyDescent="0.45">
+    <row r="56" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B56" t="s">
         <v>122</v>
       </c>
@@ -1349,7 +1349,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="57" spans="2:7" x14ac:dyDescent="0.45">
+    <row r="57" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B57" t="s">
         <v>123</v>
       </c>

</xml_diff>